<commit_message>
Actualizada secuencia de protocolo
</commit_message>
<xml_diff>
--- a/Protocolo.xlsx
+++ b/Protocolo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alesito\Documents\Programacion\CPP\Loteria_Cliente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alesito\Documents\Github\Juego-Loteria-Mexicana\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>CLIENTE 1</t>
   </si>
@@ -35,24 +35,12 @@
     <t>CLIENTE 2</t>
   </si>
   <si>
-    <t>Conectar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre </t>
-  </si>
-  <si>
     <t>OK</t>
   </si>
   <si>
-    <t>TERMINOLOGIA</t>
-  </si>
-  <si>
     <t>Realiza la conexión TCP con el servidor</t>
   </si>
   <si>
-    <t>Envia el nombre de usuario elegia para validar su disponibilidad</t>
-  </si>
-  <si>
     <t>El nombre esta disponible</t>
   </si>
   <si>
@@ -62,9 +50,6 @@
     <t>REGTAB</t>
   </si>
   <si>
-    <t>Envia los datos del tablero (Nombre y puntaje)</t>
-  </si>
-  <si>
     <t>Realizar conexión y esperar jugadores</t>
   </si>
   <si>
@@ -84,6 +69,48 @@
   </si>
   <si>
     <t>ID de la carta lanzada</t>
+  </si>
+  <si>
+    <t>Comando</t>
+  </si>
+  <si>
+    <t>Tamaño</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Envía el nombre de usuario elegido para validar su disponibilidad</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>OCUPADO</t>
+  </si>
+  <si>
+    <t>El nombre esta ocupado</t>
+  </si>
+  <si>
+    <t>CARTAS</t>
+  </si>
+  <si>
+    <t>Los 16 IDS de las cartas que conformaran la tabla del jugador</t>
+  </si>
+  <si>
+    <t>LOTERIA</t>
+  </si>
+  <si>
+    <t>GANADOR</t>
+  </si>
+  <si>
+    <t>Nombre del ganador de la partida</t>
+  </si>
+  <si>
+    <t>Envía los datos del tablero ( nombre[10] y ganados int16_t )x4</t>
+  </si>
+  <si>
+    <t>El jugador ha hecho loteria (el servidor valida su tabla contra las cartas lanzadas, por su fd sabe quien es)</t>
   </si>
 </sst>
 </file>
@@ -99,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +151,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -137,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -150,13 +183,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,100 +590,6 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="Conector recto de flecha 12"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4210050" y="2190750"/>
-          <a:ext cx="581025" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Conector recto de flecha 13"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="876300" y="2200275"/>
-          <a:ext cx="533400" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
@@ -661,7 +601,7 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Conector recto de flecha 14"/>
+        <xdr:cNvPr id="13" name="Conector recto de flecha 12"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -708,12 +648,341 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="Conector recto de flecha 15"/>
+        <xdr:cNvPr id="14" name="Conector recto de flecha 13"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
           <a:off x="876300" y="2200275"/>
+          <a:ext cx="533400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Conector recto de flecha 14"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4210050" y="2190750"/>
+          <a:ext cx="581025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Conector recto de flecha 15"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="876300" y="2200275"/>
+          <a:ext cx="533400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Conector recto de flecha 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3971925" y="2000250"/>
+          <a:ext cx="581025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Conector recto de flecha 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="762000" y="2019300"/>
+          <a:ext cx="533400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Conector recto de flecha 19"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1533525" y="2962275"/>
+          <a:ext cx="581025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Conector recto de flecha 20"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4000500" y="3152775"/>
+          <a:ext cx="581025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Conector recto de flecha 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="742950" y="3152775"/>
           <a:ext cx="533400" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -1006,23 +1275,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="94.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1031,171 +1305,261 @@
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
       <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
       <c r="G2" s="1"/>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2"/>
       <c r="G3" s="1"/>
       <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2"/>
       <c r="G4" s="1"/>
       <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
         <v>5</v>
       </c>
-      <c r="J4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2"/>
       <c r="G5" s="1"/>
       <c r="I5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="D6" s="2"/>
       <c r="F6" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="9">
+        <v>49</v>
+      </c>
+      <c r="K6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="D7" s="2"/>
       <c r="F7" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="9">
+        <v>17</v>
+      </c>
+      <c r="K7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="B9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
       <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="C10" t="s">
+      <c r="C10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10">
         <v>11</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
+      <c r="C11" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="D11" s="2"/>
+      <c r="E11" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
       <c r="D12" s="2"/>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
       <c r="D14" s="2"/>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="D15" s="2"/>
       <c r="G15" s="1"/>
-      <c r="J15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Avance a doc del protocolo
</commit_message>
<xml_diff>
--- a/Protocolo.xlsx
+++ b/Protocolo.xlsx
@@ -24,32 +24,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
-  <si>
-    <t>CLIENTE 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>SERVIDOR</t>
   </si>
   <si>
-    <t>CLIENTE 2</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>Realiza la conexión TCP con el servidor</t>
   </si>
   <si>
     <t>El nombre esta disponible</t>
   </si>
   <si>
-    <t xml:space="preserve">OK </t>
-  </si>
-  <si>
-    <t>REGTAB</t>
-  </si>
-  <si>
     <t>Realizar conexión y esperar jugadores</t>
   </si>
   <si>
@@ -62,9 +47,6 @@
     <t>CONECTAR</t>
   </si>
   <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
     <t>LANZAMIENTO</t>
   </si>
   <si>
@@ -86,18 +68,9 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>OCUPADO</t>
-  </si>
-  <si>
     <t>El nombre esta ocupado</t>
   </si>
   <si>
-    <t>CARTAS</t>
-  </si>
-  <si>
-    <t>Los 16 IDS de las cartas que conformaran la tabla del jugador</t>
-  </si>
-  <si>
     <t>LOTERIA</t>
   </si>
   <si>
@@ -107,17 +80,38 @@
     <t>Nombre del ganador de la partida</t>
   </si>
   <si>
-    <t>Envía los datos del tablero ( nombre[10] y ganados int16_t )x4</t>
-  </si>
-  <si>
     <t>El jugador ha hecho loteria (el servidor valida su tabla contra las cartas lanzadas, por su fd sabe quien es)</t>
+  </si>
+  <si>
+    <t>NOMBRE_REG</t>
+  </si>
+  <si>
+    <t>NOMBRE_OK</t>
+  </si>
+  <si>
+    <t>NOMBRE_OCUPADO</t>
+  </si>
+  <si>
+    <t>NUEVA_PARTIDA</t>
+  </si>
+  <si>
+    <t>Envía los datos del tablero ( nombre[10] y ganados int16_t )x4 y Los 16 IDS de las cartas que conformaran la tabla del jugador</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>JUGADOR 1</t>
+  </si>
+  <si>
+    <t>JUGADOR N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,8 +119,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,12 +153,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -170,10 +166,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -186,10 +180,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -213,13 +210,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
+      <xdr:colOff>819150</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -230,7 +227,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1638300" y="485775"/>
+          <a:off x="1847850" y="676275"/>
           <a:ext cx="581025" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -260,13 +257,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
+      <xdr:colOff>819150</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -277,7 +274,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1447800" y="485775"/>
+          <a:off x="1847850" y="485775"/>
           <a:ext cx="581025" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -354,15 +351,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:colOff>885825</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -371,7 +368,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3143250" y="866775"/>
+          <a:off x="3695700" y="1047750"/>
           <a:ext cx="533400" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -401,15 +398,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:colOff>885825</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -418,7 +415,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3143250" y="1076325"/>
+          <a:off x="3695700" y="1257300"/>
           <a:ext cx="533400" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -448,15 +445,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:colOff>742950</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -465,7 +462,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3857625" y="1247775"/>
+          <a:off x="4772025" y="1447800"/>
           <a:ext cx="581025" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -496,13 +493,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -542,15 +539,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -559,7 +556,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3857625" y="1600200"/>
+          <a:off x="4772025" y="2181225"/>
           <a:ext cx="581025" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -589,15 +586,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -606,7 +603,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4210050" y="2190750"/>
+          <a:off x="4781550" y="2581275"/>
           <a:ext cx="581025" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -637,13 +634,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -683,15 +680,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -700,7 +697,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4210050" y="2190750"/>
+          <a:off x="4781550" y="2962275"/>
           <a:ext cx="581025" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -731,13 +728,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -776,109 +773,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="Conector recto de flecha 16"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3971925" y="2000250"/>
-          <a:ext cx="581025" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="Conector recto de flecha 17"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="762000" y="2019300"/>
-          <a:ext cx="533400" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -918,15 +821,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -935,7 +838,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4000500" y="3152775"/>
+          <a:off x="4810125" y="3543300"/>
           <a:ext cx="581025" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -966,13 +869,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -984,6 +887,100 @@
         <a:xfrm flipH="1">
           <a:off x="742950" y="3152775"/>
           <a:ext cx="533400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>885825</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Conector recto de flecha 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3695700" y="1638300"/>
+          <a:ext cx="533400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Conector recto de flecha 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4772025" y="1828800"/>
+          <a:ext cx="581025" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1275,296 +1272,353 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="94.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="1"/>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="2"/>
+      <c r="I3" t="s">
         <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="G3" s="1"/>
-      <c r="I3" t="s">
-        <v>12</v>
       </c>
       <c r="J3">
         <v>11</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="G4" s="1"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="2"/>
       <c r="I4" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="G5" s="1"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="2"/>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="K5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="I6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="6">
+        <v>65</v>
+      </c>
+      <c r="K6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="I7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="D6" s="2"/>
-      <c r="F6" t="s">
+      <c r="F8" s="5"/>
+      <c r="G8" s="2"/>
+      <c r="I8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9">
         <v>11</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="I6" s="8" t="s">
+      <c r="K9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="8">
-        <v>49</v>
-      </c>
-      <c r="K6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="D7" s="2"/>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="I7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="8">
-        <v>17</v>
-      </c>
-      <c r="K7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="I8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="K8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="1"/>
-      <c r="I9" t="s">
+      <c r="D14" s="1"/>
+      <c r="E14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="2"/>
+      <c r="K14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="C10" s="8" t="s">
+      <c r="D15" s="1"/>
+      <c r="E15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="8" t="s">
+      <c r="D16" s="1"/>
+      <c r="E16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="I10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10">
-        <v>11</v>
-      </c>
-      <c r="K10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="C11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="G15" s="1"/>
-      <c r="K15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="1"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="2"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="2"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B21:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>